<commit_message>
added summarized test cycle details doc
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Documents\JavaTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67B682BA-B946-439D-8F38-B0F08F8F3777}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC700435-5D4F-4625-B174-496176F18E53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" activeTab="2" xr2:uid="{0AA9D21D-2CFB-48C6-85A2-7E9CC2EA4FB7}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" xr2:uid="{0AA9D21D-2CFB-48C6-85A2-7E9CC2EA4FB7}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="107">
   <si>
     <t>Users should be able to open a new User account with the Planetarium</t>
   </si>
@@ -346,10 +346,19 @@
     <t>Check-in</t>
   </si>
   <si>
-    <t>Release</t>
-  </si>
-  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Test Cycle 1 Complete + Report</t>
+  </si>
+  <si>
+    <t>In-Progress</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>To do</t>
   </si>
 </sst>
 </file>
@@ -939,8 +948,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274D401D-635C-4494-8149-60E975934667}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D6"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1686,10 +1695,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70BF23C-6DF2-4EBF-9E8D-8D2C07A7822A}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1705,7 +1714,7 @@
         <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1715,13 +1724,30 @@
       <c r="B2" s="28">
         <v>45587</v>
       </c>
+      <c r="C2" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" s="28">
+        <v>45596</v>
+      </c>
+      <c r="C3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="28">
         <v>45597</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AIO Tracability Docs added
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Documents\JavaTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85A5EB5C-9D16-4A30-A7AB-AEFB9BD1C468}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2499E173-00E0-4A4F-AF19-7C77353316AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" xr2:uid="{0AA9D21D-2CFB-48C6-85A2-7E9CC2EA4FB7}"/>
   </bookViews>
@@ -654,7 +654,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -662,7 +662,7 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
       <extLst>
         <ext xmlns:xfpb="http://schemas.microsoft.com/office/spreadsheetml/2022/featurepropertybag" uri="{C7286773-470A-42A8-94C5-96B5CB345126}">
@@ -677,25 +677,11 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1048,8 +1034,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274D401D-635C-4494-8149-60E975934667}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
In progress UX acceptance
</commit_message>
<xml_diff>
--- a/RTM.xlsx
+++ b/RTM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marce\Documents\JavaTesting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2499E173-00E0-4A4F-AF19-7C77353316AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2456AB2D-B0D1-476A-8717-F8DD287F8F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="20928" windowHeight="12552" xr2:uid="{0AA9D21D-2CFB-48C6-85A2-7E9CC2EA4FB7}"/>
+    <workbookView xWindow="10368" yWindow="0" windowWidth="10368" windowHeight="12360" xr2:uid="{0AA9D21D-2CFB-48C6-85A2-7E9CC2EA4FB7}"/>
   </bookViews>
   <sheets>
     <sheet name="RTM" sheetId="1" r:id="rId1"/>
@@ -1034,7 +1034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274D401D-635C-4494-8149-60E975934667}">
   <dimension ref="A1:H34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>

</xml_diff>